<commit_message>
Added scanning for hazards
</commit_message>
<xml_diff>
--- a/IMU_Distance_Component_Data_4_3.xlsx
+++ b/IMU_Distance_Component_Data_4_3.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://purdue0-my.sharepoint.com/personal/lcoxley_purdue_edu/Documents/ENG 162/Proj 3/Programs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0BD9333A-4932-4057-B4E6-51173A2463ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:40009_{0BD9333A-4932-4057-B4E6-51173A2463ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0D1908B6-31CE-455B-A761-0DCCF97B9141}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IMU_Distance_Component_Data_4_3" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -46,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -703,7 +714,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -867,6 +878,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mag Reading Magnitude</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -929,6 +995,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Radius (cm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -967,6 +1088,852 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1834533279"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:bubbleChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IMU_Distance_Component_Data_4_3!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>z comp Mag reading</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>IMU_Distance_Component_Data_4_3!$A$2:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IMU_Distance_Component_Data_4_3!$B$2:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>IMU_Distance_Component_Data_4_3!$H$2:$H$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>109.215</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120.595</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>141.65700000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>196.68899999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>399.66300000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>681.61900000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1824.7280000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>191.934</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>154.90600000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>127.39</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>112.273</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>178.685</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>150.32</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>133.334</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>115.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F044-4975-8723-688455FC95E8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:bubbleScale val="100"/>
+        <c:showNegBubbles val="0"/>
+        <c:axId val="1233143839"/>
+        <c:axId val="1233145087"/>
+      </c:bubbleChart>
+      <c:valAx>
+        <c:axId val="1233143839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1233145087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1233145087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1233143839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IMU_Distance_Component_Data_4_3!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>z comp Mag reading</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>IMU_Distance_Component_Data_4_3!$A$10:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IMU_Distance_Component_Data_4_3!$E$10:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-191.934</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-154.90600000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-127.39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-112.273</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-178.685</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-150.32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-133.334</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-115.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7F76-4616-B0A9-3EDB424D59DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1383314383"/>
+        <c:axId val="1383301903"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1383314383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1383301903"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1383301903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1383314383"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1062,6 +2029,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1578,20 +2625,1071 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>507023</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>175846</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>87923</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>202223</xdr:colOff>
+      <xdr:colOff>392723</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>11723</xdr:rowOff>
+      <xdr:rowOff>19343</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1611,6 +3709,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>642731</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>178904</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>139148</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58458D2B-A493-4F2D-B079-B83A52D3C6AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC107427-19B1-476B-8B7A-93F5FD1896E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1915,11 +4085,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1972,11 +4142,15 @@
       <c r="F2">
         <v>115.313</v>
       </c>
+      <c r="H2">
+        <f>ABS(E2)</f>
+        <v>109.215</v>
+      </c>
       <c r="I2">
         <v>115.313</v>
       </c>
       <c r="J2">
-        <f>SQRT(A2^2+B2^2)</f>
+        <f t="shared" ref="J2:J8" si="0">SQRT(A2^2+B2^2)</f>
         <v>30</v>
       </c>
     </row>
@@ -1999,11 +4173,15 @@
       <c r="F3">
         <v>127.932</v>
       </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H17" si="1">ABS(E3)</f>
+        <v>120.595</v>
+      </c>
       <c r="I3">
         <v>127.932</v>
       </c>
       <c r="J3">
-        <f>SQRT(A3^2+B3^2)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
@@ -2026,11 +4204,15 @@
       <c r="F4">
         <v>159.655</v>
       </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>141.65700000000001</v>
+      </c>
       <c r="I4">
         <v>159.655</v>
       </c>
       <c r="J4">
-        <f>SQRT(A4^2+B4^2)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -2053,11 +4235,15 @@
       <c r="F5">
         <v>261.25</v>
       </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>196.68899999999999</v>
+      </c>
       <c r="I5">
         <v>261.25</v>
       </c>
       <c r="J5">
-        <f>SQRT(A5^2+B5^2)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -2080,11 +4266,15 @@
       <c r="F6">
         <v>588.601</v>
       </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>399.66300000000001</v>
+      </c>
       <c r="I6">
         <v>588.601</v>
       </c>
       <c r="J6">
-        <f>SQRT(A6^2+B6^2)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -2107,11 +4297,15 @@
       <c r="F7">
         <v>989.45899999999995</v>
       </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>681.61900000000003</v>
+      </c>
       <c r="I7">
         <v>989.45899999999995</v>
       </c>
       <c r="J7">
-        <f>SQRT(A7^2+B7^2)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -2134,11 +4328,15 @@
       <c r="F8">
         <v>2396.634</v>
       </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1824.7280000000001</v>
+      </c>
       <c r="I8">
         <v>2396.634</v>
       </c>
       <c r="J8">
-        <f>SQRT(A8^2+B8^2)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -2161,6 +4359,10 @@
       <c r="F9">
         <v>0</v>
       </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -2181,11 +4383,15 @@
       <c r="F10">
         <v>281.39400000000001</v>
       </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>191.934</v>
+      </c>
       <c r="I10">
         <v>281.39400000000001</v>
       </c>
       <c r="J10">
-        <f>SQRT(A10^2+B10^2)</f>
+        <f t="shared" ref="J10:J17" si="2">SQRT(A10^2+B10^2)</f>
         <v>15.811388300841896</v>
       </c>
     </row>
@@ -2208,11 +4414,15 @@
       <c r="F11">
         <v>219.596</v>
       </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>154.90600000000001</v>
+      </c>
       <c r="I11">
         <v>219.596</v>
       </c>
       <c r="J11">
-        <f>SQRT(A11^2+B11^2)</f>
+        <f t="shared" si="2"/>
         <v>18.027756377319946</v>
       </c>
     </row>
@@ -2235,11 +4445,15 @@
       <c r="F12">
         <v>168.62899999999999</v>
       </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>127.39</v>
+      </c>
       <c r="I12">
         <v>168.62899999999999</v>
       </c>
       <c r="J12">
-        <f>SQRT(A12^2+B12^2)</f>
+        <f t="shared" si="2"/>
         <v>21.213203435596427</v>
       </c>
     </row>
@@ -2262,11 +4476,15 @@
       <c r="F13">
         <v>138.30000000000001</v>
       </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>112.273</v>
+      </c>
       <c r="I13">
         <v>138.30000000000001</v>
       </c>
       <c r="J13">
-        <f>SQRT(A13^2+B13^2)</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
     </row>
@@ -2289,11 +4507,15 @@
       <c r="F14">
         <v>249.941</v>
       </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>178.685</v>
+      </c>
       <c r="I14">
         <v>249.941</v>
       </c>
       <c r="J14">
-        <f>SQRT(A14^2+B14^2)</f>
+        <f t="shared" si="2"/>
         <v>15.811388300841896</v>
       </c>
     </row>
@@ -2316,11 +4538,15 @@
       <c r="F15">
         <v>202.744</v>
       </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>150.32</v>
+      </c>
       <c r="I15">
         <v>202.744</v>
       </c>
       <c r="J15">
-        <f>SQRT(A15^2+B15^2)</f>
+        <f t="shared" si="2"/>
         <v>18.027756377319946</v>
       </c>
     </row>
@@ -2343,11 +4569,15 @@
       <c r="F16">
         <v>164.167</v>
       </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>133.334</v>
+      </c>
       <c r="I16">
         <v>164.167</v>
       </c>
       <c r="J16">
-        <f>SQRT(A16^2+B16^2)</f>
+        <f t="shared" si="2"/>
         <v>21.213203435596427</v>
       </c>
     </row>
@@ -2370,11 +4600,15 @@
       <c r="F17">
         <v>133.00800000000001</v>
       </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>115.33</v>
+      </c>
       <c r="I17">
         <v>133.00800000000001</v>
       </c>
       <c r="J17">
-        <f>SQRT(A17^2+B17^2)</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
     </row>

</xml_diff>